<commit_message>
make 5 class and 6 class schedules
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\repos\mcnair_academic_writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C93F36-E01C-4EC2-A342-B0C118E78570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E1F0D3-C621-43AD-9353-571F1A4A5229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{44180262-F9C1-42F0-8F3A-1B9C1CDE65F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{44180262-F9C1-42F0-8F3A-1B9C1CDE65F5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="5 classes" sheetId="1" r:id="rId1"/>
+    <sheet name="6 classes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,50 +37,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Reading</t>
-  </si>
-  <si>
-    <t>Assignment Due</t>
-  </si>
-  <si>
-    <t>Writing BASE</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
     <t>Methods</t>
   </si>
   <si>
-    <t>Figures</t>
-  </si>
-  <si>
     <t>Results</t>
   </si>
   <si>
     <t>Discussion</t>
   </si>
   <si>
-    <t>Preparing to Write</t>
-  </si>
-  <si>
-    <t>What is your BASE?</t>
-  </si>
-  <si>
-    <t>Outlining</t>
-  </si>
-  <si>
-    <t>Reference Management</t>
-  </si>
-  <si>
-    <t>Homework Assigned</t>
-  </si>
-  <si>
     <t>Small Group 30-45 min</t>
   </si>
   <si>
@@ -89,10 +63,94 @@
     <t>Lecture 30-45 min</t>
   </si>
   <si>
-    <t>Course Introduction (15 min)</t>
-  </si>
-  <si>
-    <t>Why Write? (15 min)</t>
+    <t>Writing Assignment</t>
+  </si>
+  <si>
+    <t>Reviewing Assignment</t>
+  </si>
+  <si>
+    <t>Assignment Due2</t>
+  </si>
+  <si>
+    <t>Assignment Due22</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Writing BASE (30 min)</t>
+  </si>
+  <si>
+    <t>Why and How We Write? (30 min)</t>
+  </si>
+  <si>
+    <t>Introduction (30 min)</t>
+  </si>
+  <si>
+    <t>Plan your story (30 min)</t>
+  </si>
+  <si>
+    <t>Outline and Introduction</t>
+  </si>
+  <si>
+    <t>Preparing to Write (30 min)</t>
+  </si>
+  <si>
+    <t>Figure/table Draft</t>
+  </si>
+  <si>
+    <t>Small Group: Introduction</t>
+  </si>
+  <si>
+    <t>Small Group: Full Paper</t>
+  </si>
+  <si>
+    <t>Small Group: Methods</t>
+  </si>
+  <si>
+    <t>Small Group: Results</t>
+  </si>
+  <si>
+    <t>Tell your story</t>
+  </si>
+  <si>
+    <t>Dissect introductions</t>
+  </si>
+  <si>
+    <t>Dissect discussions</t>
+  </si>
+  <si>
+    <t>Potential Final Proof Review</t>
+  </si>
+  <si>
+    <t>Story sketch &amp; Outline</t>
+  </si>
+  <si>
+    <t>Small Group: Discussion</t>
+  </si>
+  <si>
+    <t>Full Paper Draft 1</t>
+  </si>
+  <si>
+    <t>Final Paper</t>
+  </si>
+  <si>
+    <t>(Optional) Final Proof Review</t>
+  </si>
+  <si>
+    <t>Dissect introductions (30 min)</t>
+  </si>
+  <si>
+    <t>Bloat and cut</t>
+  </si>
+  <si>
+    <t>Figure/Table Draft</t>
+  </si>
+  <si>
+    <t>Response to Reviews</t>
+  </si>
+  <si>
+    <t>Publish or Perish</t>
   </si>
 </sst>
 </file>
@@ -149,16 +207,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74AC054B-80FE-48EE-9219-BAE4D010BF7B}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0">
-  <autoFilter ref="A1:G1048576" xr:uid="{74AC054B-80FE-48EE-9219-BAE4D010BF7B}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74AC054B-80FE-48EE-9219-BAE4D010BF7B}" name="Table1" displayName="Table1" ref="A1:H1048574" totalsRowShown="0">
+  <autoFilter ref="A1:H1048574" xr:uid="{74AC054B-80FE-48EE-9219-BAE4D010BF7B}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{56B86EE9-6BB6-4FD0-B5EC-C4AFAD85550E}" name="Date"/>
     <tableColumn id="2" xr3:uid="{929FC5B8-24EA-48FD-AE09-D3985B541963}" name="Lecture 30-45 min"/>
     <tableColumn id="3" xr3:uid="{202954D3-DE52-4DDD-95D6-14925644F771}" name="Workshop 30-45"/>
     <tableColumn id="4" xr3:uid="{7099A444-55B1-4B51-BCFD-EDE1EF1B99E3}" name="Small Group 30-45 min"/>
-    <tableColumn id="5" xr3:uid="{6E95A466-7B7C-475E-AFAF-C331C1834B06}" name="Homework Assigned"/>
-    <tableColumn id="6" xr3:uid="{D3FF5575-D453-41DB-8244-83C37095D9E6}" name="Reading"/>
-    <tableColumn id="7" xr3:uid="{78024D31-BDBD-4221-8360-B8E9D7649E67}" name="Assignment Due"/>
+    <tableColumn id="5" xr3:uid="{6E95A466-7B7C-475E-AFAF-C331C1834B06}" name="Writing Assignment"/>
+    <tableColumn id="8" xr3:uid="{3C8A26F4-81B7-4EE3-B0CE-26BCFE4F1FC2}" name="Assignment Due2"/>
+    <tableColumn id="6" xr3:uid="{D3FF5575-D453-41DB-8244-83C37095D9E6}" name="Reviewing Assignment"/>
+    <tableColumn id="7" xr3:uid="{78024D31-BDBD-4221-8360-B8E9D7649E67}" name="Assignment Due22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71651E93-CDC4-4090-943F-30F12C236889}" name="Table13" displayName="Table13" ref="A1:H1048575" totalsRowShown="0">
+  <autoFilter ref="A1:H1048575" xr:uid="{74AC054B-80FE-48EE-9219-BAE4D010BF7B}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{CDF5AD70-F975-476C-97A4-5E7F47945C13}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{444A7D75-57CD-4880-B3B1-7F2F02132442}" name="Lecture 30-45 min"/>
+    <tableColumn id="3" xr3:uid="{4C6AE752-9985-4073-B065-77EAA0399F2A}" name="Workshop 30-45"/>
+    <tableColumn id="4" xr3:uid="{7708209C-D564-4627-A472-230138E8E704}" name="Small Group 30-45 min"/>
+    <tableColumn id="5" xr3:uid="{9B85C84B-24C7-4C75-A69C-1B434B58635B}" name="Writing Assignment"/>
+    <tableColumn id="8" xr3:uid="{16A46A26-7536-4699-9CFD-03696987625B}" name="Assignment Due2"/>
+    <tableColumn id="6" xr3:uid="{9AB31578-ED1F-448B-BB1E-3AC6A1477598}" name="Reviewing Assignment"/>
+    <tableColumn id="7" xr3:uid="{360C0566-3001-4640-9150-6C5CE61B0D7B}" name="Assignment Due22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -461,115 +537,450 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDD8D86-AF9E-497D-B095-98C06A3B0A5E}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45083</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45083</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45090</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45090</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>45097</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>45097</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45097</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>45104</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45118</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>45118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45128</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45135</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B027D88-B74D-46DB-96B0-177060A0FF6B}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45076</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45076</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45083</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45083</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1">
+        <v>45090</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45090</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>45097</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45097</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45104</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>45104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45104</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45118</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45118</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <v>45128</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>45125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45135</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>